<commit_message>
Confirm deletion: functional_form_upd (1) (2).ipynb
</commit_message>
<xml_diff>
--- a/authors_is_russian_mapping.xlsx
+++ b/authors_is_russian_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mreshetnev/Desktop/Study/Jupyter/Econometrics 2/project_books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E02DF990-13A2-AE4C-B26A-B60A6B93F8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43FDBED-0032-0A4B-B1AC-BB64D4AC7287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="2760" windowWidth="27840" windowHeight="16740" xr2:uid="{E77DF606-32A9-C540-A14C-E7492AB149B9}"/>
   </bookViews>
@@ -1973,11 +1973,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C7B05D-9103-9640-8A16-77D52F3439EC}">
   <dimension ref="A1:B521"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="A261" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>